<commit_message>
Riesgos con impacto y probabilidad
</commit_message>
<xml_diff>
--- a/Analisis de riesgos.xlsx
+++ b/Analisis de riesgos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Escritorio\Universidad\Semestre IV\Software\Proyecto\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08D6623-DE26-4423-A213-2F8E933C3E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F065D2E-DC0D-4F49-BCB5-71B20D22084B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{126D1E78-B60A-4931-B5D4-B3261A7168E0}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t>Entrega tardía, recorte de pruebas, reducción de funcionalidades y merma en la calidad final.</t>
+  </si>
+  <si>
+    <t>Riesgo2</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>Probabilidad</t>
   </si>
 </sst>
 </file>
@@ -389,7 +398,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -417,27 +435,35 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{3F062B05-7BFE-4DCC-8649-4B6FEA5F7B09}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="9" unboundColumnsRight="3">
+    <queryTableFields count="8">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
       <queryTableField id="2" name="Fase" tableColumnId="2"/>
       <queryTableField id="3" name="Riesgo" tableColumnId="3"/>
       <queryTableField id="4" name="Descripción" tableColumnId="4"/>
       <queryTableField id="5" name="Posibles consecuencias" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="8"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEEE99EA-C794-4C9B-BBDF-741C799949FF}" name="riesgo2" displayName="riesgo2" ref="A1:E30" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E30" xr:uid="{DEEE99EA-C794-4C9B-BBDF-741C799949FF}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEEE99EA-C794-4C9B-BBDF-741C799949FF}" name="riesgo2" displayName="riesgo2" ref="A1:H30" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H30" xr:uid="{DEEE99EA-C794-4C9B-BBDF-741C799949FF}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{317A9917-511A-4FEF-A911-0F5012036266}" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{06600377-2D74-4AD3-9B82-B77BD5C98911}" uniqueName="2" name="Fase" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BC904101-EE34-40E0-AEFE-732719B9E296}" uniqueName="3" name="Riesgo" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C13A56EB-A1B9-4DE0-94B6-9E25E99397DD}" uniqueName="4" name="Descripción" queryTableFieldId="4" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{7842F48F-5CC5-49F1-B0A0-3A17AA2D6809}" uniqueName="5" name="Posibles consecuencias" queryTableFieldId="5" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{06600377-2D74-4AD3-9B82-B77BD5C98911}" uniqueName="2" name="Fase" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{BC904101-EE34-40E0-AEFE-732719B9E296}" uniqueName="3" name="Riesgo" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{C13A56EB-A1B9-4DE0-94B6-9E25E99397DD}" uniqueName="4" name="Descripción" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{7842F48F-5CC5-49F1-B0A0-3A17AA2D6809}" uniqueName="5" name="Posibles consecuencias" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{8E66B3BA-C640-402E-9FE4-0039CD3AADA8}" uniqueName="6" name="Probabilidad" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{55D0F3B5-1987-4945-9382-A1C9638E0942}" uniqueName="7" name="Impacto" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{9267A347-58D2-487D-A129-5835AD3649FA}" uniqueName="8" name="Riesgo2" queryTableFieldId="8" dataDxfId="0">
+      <calculatedColumnFormula>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -760,19 +786,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBF7A43-F8EC-4347-87A0-2FC7280D1A1B}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="89.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -788,8 +819,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -805,8 +845,18 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -822,8 +872,18 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -839,8 +899,18 @@
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -856,8 +926,18 @@
       <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -873,8 +953,18 @@
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -890,8 +980,18 @@
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -907,8 +1007,18 @@
       <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -924,8 +1034,18 @@
       <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -941,8 +1061,18 @@
       <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -958,8 +1088,18 @@
       <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -975,8 +1115,18 @@
       <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -992,8 +1142,18 @@
       <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1009,8 +1169,18 @@
       <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1026,8 +1196,18 @@
       <c r="E15" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1043,8 +1223,18 @@
       <c r="E16" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1060,8 +1250,18 @@
       <c r="E17" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1077,8 +1277,18 @@
       <c r="E18" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1094,8 +1304,18 @@
       <c r="E19" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
+      <c r="H19" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1111,8 +1331,18 @@
       <c r="E20" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>3</v>
+      </c>
+      <c r="H20" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1128,8 +1358,18 @@
       <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1145,8 +1385,18 @@
       <c r="E22" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1">
+        <v>4</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1162,8 +1412,18 @@
       <c r="E23" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1179,8 +1439,18 @@
       <c r="E24" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1196,8 +1466,18 @@
       <c r="E25" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>5</v>
+      </c>
+      <c r="H25" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1213,8 +1493,18 @@
       <c r="E26" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1230,8 +1520,18 @@
       <c r="E27" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1247,8 +1547,18 @@
       <c r="E28" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1264,8 +1574,18 @@
       <c r="E29" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1280,6 +1600,16 @@
       </c>
       <c r="E30" s="1" t="s">
         <v>99</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>5</v>
+      </c>
+      <c r="H30" s="1">
+        <f>riesgo2[[#This Row],[Probabilidad]]*riesgo2[[#This Row],[Impacto]]</f>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>